<commit_message>
Update for Aug 2025
</commit_message>
<xml_diff>
--- a/code/inputs/landmarks.xlsx
+++ b/code/inputs/landmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengzeng/Documents/Brown/GIS/geodata_pvdcrime/code/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\_geodata\data_public\providence_crime\geodata_pvdcrime\code\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406E26EA-D0E9-EE43-945F-8EAB7A24D5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94094012-72F6-4CDF-B3ED-E56931DA59CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="4280" windowWidth="23260" windowHeight="12460" xr2:uid="{330E0894-3643-48AB-9E2C-CEE2BA7238FE}"/>
+    <workbookView xWindow="10200" yWindow="4284" windowWidth="23256" windowHeight="12456" xr2:uid="{330E0894-3643-48AB-9E2C-CEE2BA7238FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>location</t>
   </si>
@@ -298,13 +298,40 @@
   </si>
   <si>
     <t>CALHOUN</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>S CHARLES 104</t>
+  </si>
+  <si>
+    <t>ELMWOOD ST PROVIDENCE</t>
+  </si>
+  <si>
+    <t>ANNE</t>
+  </si>
+  <si>
+    <t>FEDERAL HILL</t>
+  </si>
+  <si>
+    <t>NPA</t>
+  </si>
+  <si>
+    <t>UNAVAILABLE CT</t>
+  </si>
+  <si>
+    <t>MARKET ST 10TH</t>
+  </si>
+  <si>
+    <t>BROADWAY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,9 +389,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -402,7 +429,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -508,7 +535,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,20 +685,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E20005D-6A1D-449E-93B2-CD2D6060E071}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -699,7 +726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -713,7 +740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -727,7 +754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -741,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -755,7 +782,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -769,7 +796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -780,7 +807,7 @@
         <v>-71.435100000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -794,7 +821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -805,7 +832,7 @@
         <v>-71.412949999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -819,7 +846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -833,7 +860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -844,7 +871,7 @@
         <v>-71.466279999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -855,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -866,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -877,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -888,7 +915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -899,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -910,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -921,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -932,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -943,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -954,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -965,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -976,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -987,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -998,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1012,7 +1039,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1023,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1037,7 +1064,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1048,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1059,7 +1086,7 @@
         <v>-71.412009999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1070,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1081,7 +1108,7 @@
         <v>-71.410160000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1092,7 +1119,7 @@
         <v>-71.417460000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1103,7 +1130,7 @@
         <v>-71.407640000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1117,7 +1144,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1128,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1142,7 +1169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
@@ -1153,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
@@ -1164,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -1175,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -1186,7 +1213,7 @@
         <v>-71.407229999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1197,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -1208,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -1219,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -1230,7 +1257,7 @@
         <v>-71.410880000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
@@ -1241,9 +1268,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1252,9 +1279,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1263,9 +1290,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1274,9 +1301,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1284,10 +1311,13 @@
       <c r="C52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D52" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1295,13 +1325,10 @@
       <c r="C53">
         <v>0</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1310,9 +1337,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1321,9 +1348,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1332,9 +1359,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1343,31 +1370,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>41.817880000000002</v>
       </c>
       <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>-71.403670000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59">
-        <v>41.817880000000002</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>-71.403670000000005</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -1376,9 +1403,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -1387,9 +1414,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -1398,9 +1425,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -1409,67 +1436,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>41.80941</v>
       </c>
       <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>-71.440060000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B65">
-        <v>41.80941</v>
+        <v>41.830047</v>
       </c>
       <c r="C65">
-        <v>-71.440060000000003</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>-71.400886999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B66">
-        <v>41.830047</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>-71.400886999999997</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>41.822938000000001</v>
       </c>
       <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>78</v>
+        <v>-71.418092999999999</v>
+      </c>
+      <c r="D67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>80</v>
       </c>
       <c r="B68">
-        <v>41.822938000000001</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>-71.418092999999999</v>
-      </c>
-      <c r="D68" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -1478,9 +1505,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1489,9 +1516,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1500,9 +1527,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -1511,9 +1538,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1522,9 +1549,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -1533,14 +1560,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
         <v>0</v>
       </c>
     </row>

</xml_diff>